<commit_message>
Subiendo a productivo priorizar
</commit_message>
<xml_diff>
--- a/docs/CodeSystem-CSPractitionerTipoRolLE.xlsx
+++ b/docs/CodeSystem-CSPractitionerTipoRolLE.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
   <si>
     <t>Property</t>
   </si>
@@ -123,7 +123,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>6</t>
+    <t>7</t>
   </si>
   <si>
     <t>Level</t>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>Revisor</t>
+  </si>
+  <si>
+    <t>priorizador</t>
+  </si>
+  <si>
+    <t>Priorizador</t>
   </si>
   <si>
     <t>agendador</t>
@@ -487,7 +493,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -579,6 +585,18 @@
       </c>
       <c r="D7" s="2"/>
     </row>
+    <row r="8">
+      <c r="A8" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>